<commit_message>
Deploying to gh-pages from  @ 8a1399b77229fd6f0fb7a0b56e17a25ca43ef4c2 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_4-1-5.xlsx
+++ b/assets/excel/2021_4-1-5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60331E8B-B175-4943-A671-786D7E731C57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FC72A2-4115-4567-A118-E22DB41C7DCD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{1669E68D-AC48-46B3-BA56-D23CBC6394FE}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="37">
   <si>
     <t>Migration und Teilhabe in Niedersachsen - Integrationsmonitoring 2021</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>https://www.integrationsmonitoring.niedersachsen.de</t>
+  </si>
+  <si>
+    <t>Migrationsstatus</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -606,6 +609,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -648,12 +660,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -666,7 +672,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -989,7 +995,7 @@
   <dimension ref="B1:V168"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B9"/>
+      <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,8 +1005,7 @@
     <col min="3" max="3" width="11.5703125" style="2" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="3" customWidth="1"/>
     <col min="5" max="5" width="8.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="5.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" style="2" customWidth="1"/>
+    <col min="6" max="7" width="7.7109375" style="2" customWidth="1"/>
     <col min="8" max="11" width="5.7109375" style="2" customWidth="1"/>
     <col min="12" max="16384" width="11.42578125" style="2"/>
   </cols>
@@ -1042,58 +1047,60 @@
       <c r="L4" s="10"/>
     </row>
     <row r="6" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="40" t="s">
+      <c r="B6" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="43" t="s">
+      <c r="F6" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="59"/>
+    </row>
+    <row r="7" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="44"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="52" t="s">
+      <c r="G7" s="39" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="41"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="53"/>
-    </row>
     <row r="8" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="41"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="54" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="55"/>
+      <c r="G8" s="56"/>
     </row>
     <row r="9" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="42"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="56" t="s">
+      <c r="B9" s="45"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="58"/>
     </row>
     <row r="10" spans="2:12" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="58">
+      <c r="B10" s="40">
         <v>1</v>
       </c>
-      <c r="C10" s="58">
+      <c r="C10" s="40">
         <v>2</v>
       </c>
       <c r="D10" s="16">
@@ -4480,18 +4487,18 @@
       <c r="B156" s="25"/>
     </row>
     <row r="157" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B157" s="38" t="s">
+      <c r="B157" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C157" s="38"/>
-      <c r="D157" s="38"/>
-      <c r="E157" s="38"/>
-      <c r="F157" s="38"/>
-      <c r="G157" s="38"/>
-      <c r="H157" s="38"/>
-      <c r="I157" s="38"/>
-      <c r="J157" s="38"/>
-      <c r="K157" s="38"/>
+      <c r="C157" s="41"/>
+      <c r="D157" s="41"/>
+      <c r="E157" s="41"/>
+      <c r="F157" s="41"/>
+      <c r="G157" s="41"/>
+      <c r="H157" s="41"/>
+      <c r="I157" s="41"/>
+      <c r="J157" s="41"/>
+      <c r="K157" s="41"/>
     </row>
     <row r="158" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="26" t="s">
@@ -4508,26 +4515,26 @@
       <c r="K158" s="29"/>
     </row>
     <row r="159" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B159" s="39" t="s">
+      <c r="B159" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C159" s="39"/>
-      <c r="D159" s="39"/>
-      <c r="E159" s="39"/>
-      <c r="F159" s="39"/>
-      <c r="G159" s="39"/>
+      <c r="C159" s="42"/>
+      <c r="D159" s="42"/>
+      <c r="E159" s="42"/>
+      <c r="F159" s="42"/>
+      <c r="G159" s="42"/>
       <c r="H159" s="27"/>
       <c r="I159" s="29"/>
       <c r="J159" s="29"/>
       <c r="K159" s="29"/>
     </row>
     <row r="160" spans="2:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B160" s="39"/>
-      <c r="C160" s="39"/>
-      <c r="D160" s="39"/>
-      <c r="E160" s="39"/>
-      <c r="F160" s="39"/>
-      <c r="G160" s="39"/>
+      <c r="B160" s="42"/>
+      <c r="C160" s="42"/>
+      <c r="D160" s="42"/>
+      <c r="E160" s="42"/>
+      <c r="F160" s="42"/>
+      <c r="G160" s="42"/>
       <c r="H160" s="27"/>
       <c r="I160" s="29"/>
       <c r="J160" s="29"/>
@@ -4593,17 +4600,16 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="9">
     <mergeCell ref="B157:K157"/>
     <mergeCell ref="B159:G160"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C6:C9"/>
     <mergeCell ref="D6:D9"/>
     <mergeCell ref="E6:E8"/>
-    <mergeCell ref="F6:F7"/>
-    <mergeCell ref="G6:G7"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="E9:G9"/>
+    <mergeCell ref="F6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B168" r:id="rId1" xr:uid="{8BC02B56-05EF-4E38-971F-9589A4E32309}"/>

</xml_diff>